<commit_message>
chore: initial commit 🎉
</commit_message>
<xml_diff>
--- a/public/templates/professors_template.xlsx
+++ b/public/templates/professors_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Smart Nursing Platform\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923ECB94-1DAE-4F7A-B84C-301074ABFDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED653C7-9D2C-465C-A935-CD2775147F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,31 +27,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>الجنس</t>
-  </si>
-  <si>
-    <t>الاميل</t>
-  </si>
-  <si>
-    <t>ملاحظات</t>
-  </si>
-  <si>
-    <t>الاسم الأستاذ</t>
-  </si>
-  <si>
-    <t>المرتبة العلمية</t>
-  </si>
-  <si>
-    <t>الكلية</t>
-  </si>
-  <si>
-    <t>القسم</t>
-  </si>
-  <si>
-    <t>مجالات الاهتمام</t>
-  </si>
-  <si>
-    <t>الهاتف</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>academic_rank</t>
+  </si>
+  <si>
+    <t>college</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>research_interests</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -125,6 +125,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -159,20 +173,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -187,18 +187,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7896CEA6-281F-464F-92FA-F92370A5F5C2}" name="الجدول1" displayName="الجدول1" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:I2" xr:uid="{7896CEA6-281F-464F-92FA-F92370A5F5C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7896CEA6-281F-464F-92FA-F92370A5F5C2}" name="الجدول1" displayName="الجدول1" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{AB62F554-DFC7-4856-8DF0-B2F6E9B5D016}" name="الاسم الأستاذ"/>
-    <tableColumn id="2" xr3:uid="{84B01614-809D-4054-8DDA-19AFA2CC251A}" name="الجنس"/>
-    <tableColumn id="3" xr3:uid="{67635B37-A50D-48D8-A00C-C78489939258}" name="المرتبة العلمية"/>
-    <tableColumn id="4" xr3:uid="{F1B8FE98-2BED-4761-8D4E-47166BFFFE61}" name="الكلية"/>
-    <tableColumn id="5" xr3:uid="{2D542C27-B602-4795-B374-44D26258AB5E}" name="القسم"/>
-    <tableColumn id="6" xr3:uid="{1480946B-CC78-4FFB-B9E2-051307246E74}" name="مجالات الاهتمام"/>
-    <tableColumn id="7" xr3:uid="{C24003C1-42BC-4D27-BACF-60F7479F55B7}" name="الهاتف"/>
-    <tableColumn id="8" xr3:uid="{6E6BEB84-4F19-4F53-8E03-787B8D547F31}" name="الاميل"/>
-    <tableColumn id="10" xr3:uid="{CB122843-E3A8-4B85-B11D-B079F12DFE45}" name="ملاحظات"/>
+    <tableColumn id="1" xr3:uid="{AB62F554-DFC7-4856-8DF0-B2F6E9B5D016}" name="name"/>
+    <tableColumn id="2" xr3:uid="{84B01614-809D-4054-8DDA-19AFA2CC251A}" name="gender"/>
+    <tableColumn id="3" xr3:uid="{67635B37-A50D-48D8-A00C-C78489939258}" name="academic_rank"/>
+    <tableColumn id="4" xr3:uid="{F1B8FE98-2BED-4761-8D4E-47166BFFFE61}" name="college"/>
+    <tableColumn id="5" xr3:uid="{2D542C27-B602-4795-B374-44D26258AB5E}" name="department"/>
+    <tableColumn id="6" xr3:uid="{1480946B-CC78-4FFB-B9E2-051307246E74}" name="research_interests"/>
+    <tableColumn id="7" xr3:uid="{C24003C1-42BC-4D27-BACF-60F7479F55B7}" name="phone"/>
+    <tableColumn id="8" xr3:uid="{6E6BEB84-4F19-4F53-8E03-787B8D547F31}" name="email"/>
+    <tableColumn id="10" xr3:uid="{CB122843-E3A8-4B85-B11D-B079F12DFE45}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -470,46 +469,49 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="18.25" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>